<commit_message>
stats now stored in classes for better readability
</commit_message>
<xml_diff>
--- a/assets/excel/backups/ping_pong_scoresheet_v2_formatted.xlsx
+++ b/assets/excel/backups/ping_pong_scoresheet_v2_formatted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/ping_pong/assets/excel/backups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48209E96-FBF3-3749-88E0-B6186D3ECFF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678D3187-ECF1-D041-A80C-DC84D38696C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="22200" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="24420" windowHeight="13340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +132,16 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,18 +168,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6D5A9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD6D5A9"/>
+        <fgColor rgb="FFFFD400"/>
         <bgColor theme="6" tint="-0.24994659260841701"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -234,10 +236,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="double">
+        <color rgb="FFAB1500"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -247,40 +249,51 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color rgb="FFD4D4D4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -292,9 +305,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FFAB1500"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -303,12 +314,63 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FFAB1500"/>
+      </right>
+      <top/>
+      <bottom style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="double">
         <color rgb="FFAB1500"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
       </bottom>
       <diagonal/>
     </border>
@@ -316,11 +378,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FFAB1500"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FFD4D4D4"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -329,20 +389,129 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FFAB1500"/>
+      <right/>
+      <top style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD4D4D4"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top/>
+      <bottom style="slantDashDot">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFAB1500"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFAB1500"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,64 +525,92 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1038,15 +1235,15 @@
   <colors>
     <mruColors>
       <color rgb="FFAB1500"/>
+      <color rgb="FFD4D4D4"/>
+      <color rgb="FFFFD400"/>
+      <color rgb="FF948A54"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFFE799"/>
+      <color rgb="FFFFF5D6"/>
       <color rgb="FF76D5D6"/>
       <color rgb="FFFFFDA9"/>
       <color rgb="FFD9E1F1"/>
-      <color rgb="FF4674C1"/>
-      <color rgb="FFD6D5A9"/>
-      <color rgb="FFFFD400"/>
-      <color rgb="FFD7A841"/>
-      <color rgb="FF3CA779"/>
-      <color rgb="FFFFFFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1381,15 +1578,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9.1640625" style="1"/>
+    <col min="1" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2064,7 +2264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>43405</v>
       </c>
@@ -2078,7 +2278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>43405</v>
       </c>
@@ -2092,7 +2292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>43405</v>
       </c>
@@ -2106,7 +2306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43409</v>
       </c>
@@ -2120,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>43409</v>
       </c>
@@ -2134,7 +2334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>43409</v>
       </c>
@@ -2148,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>43409</v>
       </c>
@@ -2162,7 +2362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>43409</v>
       </c>
@@ -2176,7 +2376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>43410</v>
       </c>
@@ -2190,7 +2390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>43410</v>
       </c>
@@ -2204,7 +2404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>43410</v>
       </c>
@@ -2218,7 +2418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>43410</v>
       </c>
@@ -2231,8 +2431,10 @@
       <c r="D60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F60" s="30"/>
+      <c r="G60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>43410</v>
       </c>
@@ -2245,152 +2447,168 @@
       <c r="D61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="9" t="s">
+      <c r="E61" s="14"/>
+      <c r="F61" s="31"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="14"/>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="23" t="s">
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="20">
+      <c r="C64" s="9">
         <v>14</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D64" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="21">
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="36"/>
+      <c r="B65" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="19">
         <v>11</v>
       </c>
-      <c r="D65" s="12">
+      <c r="D65" s="20">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="25"/>
-      <c r="B66" s="8" t="s">
+      <c r="E65" s="14"/>
+      <c r="G65" s="15"/>
+    </row>
+    <row r="66" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="37"/>
+      <c r="B66" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="13">
+      <c r="C66" s="21">
         <v>25</v>
       </c>
-      <c r="D66" s="14">
+      <c r="D66" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="23" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="18">
+      <c r="C67" s="10">
         <v>46.67</v>
       </c>
-      <c r="D67" s="15">
+      <c r="D67" s="7">
         <v>47.62</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="24"/>
-      <c r="B68" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="19">
+      <c r="G67" s="13"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="36"/>
+      <c r="B68" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="17">
         <v>52.38</v>
       </c>
-      <c r="D68" s="16">
+      <c r="D68" s="18">
         <v>53.33</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="25"/>
-      <c r="B69" s="7" t="s">
+    <row r="69" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="37"/>
+      <c r="B69" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="22">
+      <c r="C69" s="23">
         <v>49.02</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="24">
         <v>50.98</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="23" t="s">
+      <c r="G69" s="15"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C70" s="10">
         <v>13.17</v>
       </c>
-      <c r="D70" s="15">
+      <c r="D70" s="8">
         <v>13.62</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="19">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="36"/>
+      <c r="B71" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="17">
         <v>13.24</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="18">
         <v>13.57</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" s="7" t="s">
+    <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="37"/>
+      <c r="B72" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="22">
+      <c r="C72" s="23">
         <v>13.2</v>
       </c>
-      <c r="D72" s="17">
+      <c r="D72" s="24">
         <v>13.59</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="26" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="18">
+      <c r="C73" s="10">
         <v>0</v>
       </c>
-      <c r="D73" s="15">
+      <c r="D73" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="26"/>
-      <c r="B74" s="10" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="40"/>
+      <c r="B74" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C74" s="18">
+      <c r="C74" s="10">
         <v>0</v>
       </c>
-      <c r="D74" s="15">
+      <c r="D74" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2402,512 +2620,512 @@
     <mergeCell ref="A73:A74"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="101" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="19" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="100" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="21" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="99" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="23" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="98" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="25" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="97" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="27" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="96" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="29" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="95" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="31" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="94" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="33" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="93" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="35" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="92" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="37" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="91" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="90" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="39" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="89" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="41" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="88" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="43" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="87" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="45" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="86" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="47" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="85" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="49" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="84" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="51" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="83" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="53" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="82" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="55" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="81" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="57" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="80" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="5" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="79" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="59" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="cellIs" dxfId="78" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="61" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="77" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="63" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="cellIs" dxfId="76" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="65" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="75" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="67" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="74" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="73" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="71" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="cellIs" dxfId="72" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="71" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="70" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="77" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="69" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="7" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="68" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="79" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="cellIs" dxfId="67" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="81" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="66" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="83" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="65" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="85" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="64" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="87" operator="greaterThan">
       <formula>19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="63" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="89" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="62" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="91" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="61" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="93" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="60" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="95" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="59" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="97" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="58" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="9" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" dxfId="57" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="99" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="56" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="101" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="55" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="103" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="11" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="53" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="52" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="15" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="51" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="20" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="49" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="22" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="48" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="47" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="26" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="28" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="45" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="30" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="44" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="32" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="43" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="36" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="46" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="48" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="34" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="50" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="33" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="52" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="32" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="54" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="31" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="56" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="30" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="58" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="28" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="60" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="27" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="62" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="26" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="64" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="25" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="66" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="24" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="68" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="23" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="70" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="22" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="72" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="21" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="74" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="20" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="76" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="19" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="78" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="17" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="80" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="16" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="82" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="15" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="84" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="14" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="86" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="13" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="88" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="12" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="90" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="11" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="92" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="10" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="94" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="9" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="96" operator="greaterThan">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="8" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="98" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="6" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="100" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="5" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="102" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="4" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="104" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>